<commit_message>
All campuses included in Sports
</commit_message>
<xml_diff>
--- a/Soccer_final.xlsx
+++ b/Soccer_final.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C273"/>
+  <dimension ref="A1:C275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,7 +377,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>079</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -394,7 +394,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>079</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -411,7 +411,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>079</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -428,7 +428,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>079</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -445,12 +445,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>002</t>
+          <t>372</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -462,7 +462,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>002</t>
+          <t>056</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -479,12 +479,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>002</t>
+          <t>056</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -496,12 +496,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>002</t>
+          <t>158</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -513,12 +513,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>003</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -530,12 +530,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>003</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -547,12 +547,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>004</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -564,12 +564,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>004</t>
+          <t>248</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -581,12 +581,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>006</t>
+          <t>248</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -598,12 +598,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>006</t>
+          <t>248</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -615,12 +615,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>007</t>
+          <t>196</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -632,12 +632,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>007</t>
+          <t>267</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -649,12 +649,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>008</t>
+          <t>267</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -666,12 +666,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>008</t>
+          <t>045</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -683,12 +683,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>009</t>
+          <t>045</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -700,12 +700,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>009</t>
+          <t>045</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -717,12 +717,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>009</t>
+          <t>006</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -734,12 +734,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>009</t>
+          <t>006</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -751,12 +751,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>010</t>
+          <t>265</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -768,12 +768,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>010</t>
+          <t>225</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -785,12 +785,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>475</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -802,12 +802,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>353</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -819,12 +819,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>012</t>
+          <t>353</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -836,12 +836,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>012</t>
+          <t>075</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -853,12 +853,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>014</t>
+          <t>075</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -870,12 +870,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>014</t>
+          <t>019</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -887,12 +887,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>015</t>
+          <t>019</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -904,12 +904,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>015</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -921,7 +921,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>016</t>
+          <t>072</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>016</t>
+          <t>072</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -955,12 +955,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>017</t>
+          <t>276</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>017</t>
+          <t>024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -989,12 +989,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>018</t>
+          <t>024</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1006,12 +1006,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>018</t>
+          <t>109</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1023,12 +1023,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>217</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1040,12 +1040,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>217</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1057,12 +1057,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>020</t>
+          <t>262</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1074,12 +1074,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>020</t>
+          <t>262</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1091,12 +1091,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>023</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1108,12 +1108,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>023</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1125,12 +1125,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>024</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1142,12 +1142,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>024</t>
+          <t>170</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1159,7 +1159,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>026</t>
+          <t>344</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1176,12 +1176,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>027</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1193,12 +1193,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>027</t>
+          <t>159</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1210,12 +1210,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>034</t>
+          <t>159</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1227,12 +1227,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>034</t>
+          <t>159</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1244,12 +1244,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>034</t>
+          <t>082</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1261,12 +1261,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>036</t>
+          <t>082</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1278,12 +1278,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>036</t>
+          <t>182</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1295,7 +1295,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>039</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1312,7 +1312,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>039</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1329,12 +1329,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>041</t>
+          <t>153</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1346,12 +1346,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>041</t>
+          <t>153</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1363,12 +1363,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>042</t>
+          <t>308</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1380,12 +1380,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>042</t>
+          <t>308</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>sports_uil_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1397,7 +1397,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>043</t>
+          <t>077</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1414,12 +1414,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>043</t>
+          <t>264</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1431,7 +1431,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>044</t>
+          <t>018</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1448,12 +1448,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>045</t>
+          <t>018</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1465,12 +1465,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>045</t>
+          <t>268</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1482,12 +1482,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>045</t>
+          <t>268</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1499,12 +1499,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>046</t>
+          <t>231</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1516,12 +1516,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>046</t>
+          <t>383</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1533,12 +1533,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>047</t>
+          <t>098</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1550,12 +1550,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>047</t>
+          <t>098</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1567,12 +1567,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>048</t>
+          <t>486</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1584,12 +1584,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>048</t>
+          <t>486</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1601,12 +1601,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>049</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>049</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1635,12 +1635,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>050</t>
+          <t>099</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1652,12 +1652,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>050</t>
+          <t>099</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1669,7 +1669,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>051</t>
+          <t>078</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1686,7 +1686,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>051</t>
+          <t>078</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1703,12 +1703,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>052</t>
+          <t>113</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1720,12 +1720,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>052</t>
+          <t>011</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1737,12 +1737,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>053</t>
+          <t>011</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1754,12 +1754,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>053</t>
+          <t>124</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1771,7 +1771,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>053</t>
+          <t>124</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1788,12 +1788,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>053</t>
+          <t>042</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1805,12 +1805,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>054</t>
+          <t>042</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_coed</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1822,7 +1822,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>054</t>
+          <t>043</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1839,7 +1839,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>054</t>
+          <t>043</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1856,12 +1856,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>055</t>
+          <t>254</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1873,12 +1873,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>055</t>
+          <t>047</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1890,7 +1890,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>056</t>
+          <t>047</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1907,12 +1907,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>056</t>
+          <t>258</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -1924,12 +1924,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>057</t>
+          <t>258</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -1941,12 +1941,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>057</t>
+          <t>258</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -1958,12 +1958,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>059</t>
+          <t>187</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -1975,12 +1975,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>059</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -1992,12 +1992,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>060</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2009,12 +2009,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>060</t>
+          <t>023</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2026,12 +2026,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>061</t>
+          <t>023</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2043,12 +2043,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>061</t>
+          <t>274</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2060,12 +2060,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>062</t>
+          <t>321</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2077,12 +2077,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>062</t>
+          <t>163</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2094,7 +2094,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>064</t>
+          <t>039</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2111,7 +2111,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>064</t>
+          <t>039</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2128,12 +2128,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>068</t>
+          <t>311</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2145,12 +2145,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>068</t>
+          <t>324</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2162,12 +2162,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>072</t>
+          <t>324</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2179,12 +2179,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>072</t>
+          <t>044</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2196,12 +2196,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>075</t>
+          <t>136</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2213,12 +2213,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>075</t>
+          <t>136</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2230,12 +2230,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>077</t>
+          <t>136</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2247,12 +2247,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>078</t>
+          <t>136</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_coed</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>078</t>
+          <t>112</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2281,7 +2281,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>079</t>
+          <t>195</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2298,12 +2298,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>079</t>
+          <t>166</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2315,7 +2315,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>079</t>
+          <t>166</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2332,12 +2332,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>079</t>
+          <t>227</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2349,12 +2349,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>080</t>
+          <t>227</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2366,12 +2366,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>080</t>
+          <t>010</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2383,12 +2383,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>081</t>
+          <t>010</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2400,12 +2400,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>081</t>
+          <t>263</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2417,12 +2417,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>082</t>
+          <t>175</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2434,12 +2434,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>082</t>
+          <t>015</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2451,12 +2451,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>098</t>
+          <t>015</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2468,12 +2468,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>098</t>
+          <t>008</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2485,12 +2485,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>008</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2502,12 +2502,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>162</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2519,12 +2519,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>162</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2536,12 +2536,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>289</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2553,12 +2553,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>289</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2570,12 +2570,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>061</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2587,12 +2587,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>061</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2604,12 +2604,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>007</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2621,12 +2621,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>007</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -2638,12 +2638,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>052</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2655,12 +2655,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>052</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -2672,12 +2672,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>458</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2689,7 +2689,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>359</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2706,7 +2706,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2723,7 +2723,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2740,12 +2740,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -2757,12 +2757,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>sports_uil_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -2774,7 +2774,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>132</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2791,7 +2791,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>132</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2808,12 +2808,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>041</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2825,12 +2825,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>041</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -2842,12 +2842,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>476</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -2859,12 +2859,12 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>476</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_coed</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2876,7 +2876,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>485</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -2893,12 +2893,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>048</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>048</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -2927,12 +2927,12 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>192</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -2944,12 +2944,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>192</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -2961,12 +2961,12 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>053</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -2978,12 +2978,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>053</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -2995,12 +2995,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>162</t>
+          <t>053</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3012,12 +3012,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>162</t>
+          <t>053</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3029,12 +3029,12 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>046</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3046,12 +3046,12 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>046</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3063,12 +3063,12 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>020</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3080,12 +3080,12 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>020</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3097,12 +3097,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>256</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3114,7 +3114,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>256</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3131,12 +3131,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>212</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3148,12 +3148,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>212</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3165,7 +3165,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>188</t>
+          <t>212</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -3182,12 +3182,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>240</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3199,12 +3199,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>064</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3216,12 +3216,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>064</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3233,12 +3233,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>196</t>
+          <t>014</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3250,12 +3250,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>014</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3267,12 +3267,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>151</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3284,12 +3284,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>054</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3301,12 +3301,12 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>054</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3318,12 +3318,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>054</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3335,12 +3335,12 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>009</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3352,12 +3352,12 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>009</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3369,12 +3369,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>009</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3386,12 +3386,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>009</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3403,12 +3403,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>188</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3420,12 +3420,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>102</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3437,12 +3437,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>057</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3454,12 +3454,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>057</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3471,12 +3471,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>310</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3488,12 +3488,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>310</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -3505,12 +3505,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>050</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3522,12 +3522,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>050</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3539,12 +3539,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>049</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>049</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -3573,12 +3573,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>080</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3590,12 +3590,12 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>080</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -3607,7 +3607,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>001</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -3624,12 +3624,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>001</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3641,12 +3641,12 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>001</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -3658,12 +3658,12 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>001</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3675,24 +3675,14 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>256</t>
-        </is>
-      </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>sports_club_boys</t>
-        </is>
-      </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>Cheer/Drill</t>
+          <t xml:space="preserve"> NA</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>292</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -3709,7 +3699,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>468</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3726,12 +3716,12 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>016</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3743,12 +3733,12 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>016</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3760,7 +3750,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>286</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -3777,7 +3767,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>286</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -3794,12 +3784,12 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>263</t>
+          <t>036</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -3811,12 +3801,12 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>264</t>
+          <t>036</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3828,12 +3818,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>265</t>
+          <t>395</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -3845,12 +3835,12 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>003</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -3862,12 +3852,12 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>003</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -3879,7 +3869,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>268</t>
+          <t>138</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -3896,7 +3886,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>268</t>
+          <t>138</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -3913,12 +3903,12 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>274</t>
+          <t>012</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -3930,12 +3920,12 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>276</t>
+          <t>012</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -3947,12 +3937,12 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>279</t>
+          <t>105</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -3964,12 +3954,12 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>279</t>
+          <t>338</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -3981,12 +3971,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>286</t>
+          <t>338</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -3998,12 +3988,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>286</t>
+          <t>060</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -4015,12 +4005,12 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>289</t>
+          <t>060</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -4032,12 +4022,12 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>289</t>
+          <t>055</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -4049,12 +4039,12 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>055</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -4066,12 +4056,12 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>169</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4083,12 +4073,12 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>027</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -4100,12 +4090,12 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>027</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4117,12 +4107,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>237</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4134,12 +4124,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>059</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -4151,12 +4141,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>059</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4168,12 +4158,12 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>244</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -4185,12 +4175,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>244</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -4202,12 +4192,12 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>337</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4219,12 +4209,12 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>310</t>
+          <t>337</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -4236,12 +4226,12 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>310</t>
+          <t>026</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -4253,7 +4243,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>311</t>
+          <t>323</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -4270,12 +4260,12 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>323</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -4287,12 +4277,12 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>322</t>
+          <t>218</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>sports_uil_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -4304,12 +4294,12 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>323</t>
+          <t>218</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4321,12 +4311,12 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>323</t>
+          <t>002</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -4338,12 +4328,12 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>324</t>
+          <t>002</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -4355,7 +4345,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>324</t>
+          <t>002</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -4372,12 +4362,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>002</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -4389,12 +4379,12 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>290</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -4406,12 +4396,12 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>290</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -4423,12 +4413,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>062</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4440,12 +4430,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>062</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -4457,12 +4447,12 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -4474,12 +4464,12 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -4491,12 +4481,12 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>322</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_coed</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -4508,12 +4498,12 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>344</t>
+          <t>198</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -4525,7 +4515,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>147</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -4542,7 +4532,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>147</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4559,12 +4549,12 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>147</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -4576,12 +4566,12 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>004</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -4593,12 +4583,12 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>004</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -4610,12 +4600,12 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>353</t>
+          <t>051</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -4627,12 +4617,12 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>353</t>
+          <t>051</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4644,12 +4634,12 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>359</t>
+          <t>034</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4661,12 +4651,12 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>034</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4678,7 +4668,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>383</t>
+          <t>034</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -4695,12 +4685,12 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>081</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4712,12 +4702,12 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>081</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -4729,7 +4719,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>017</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -4746,12 +4736,12 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>017</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>sports_club_girls</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -4763,12 +4753,12 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>068</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>sports_uil_girls</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -4780,12 +4770,12 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>395</t>
+          <t>068</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -4797,12 +4787,12 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>458</t>
+          <t>128</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -4848,12 +4838,12 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>389</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -4865,12 +4855,12 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>297</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -4882,12 +4872,12 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>476</t>
+          <t>297</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>sports_uil_boys</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -4899,12 +4889,12 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>476</t>
+          <t>297</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>sports_uil_coed</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -4916,7 +4906,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>477</t>
+          <t>279</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -4933,7 +4923,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>477</t>
+          <t>279</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -4950,12 +4940,12 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>485</t>
+          <t>477</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>sports_club_coed</t>
+          <t>sports_uil_boys</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -4967,12 +4957,12 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>486</t>
+          <t>477</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>sports_club_boys</t>
+          <t>sports_uil_girls</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -4984,15 +4974,49 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>486</t>
+          <t>234</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
+          <t>sports_club_boys</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Cheer/Drill</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
           <t>sports_club_girls</t>
         </is>
       </c>
-      <c r="C273" t="inlineStr">
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Cheer/Drill</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>sports_club_coed</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
         <is>
           <t>Cheer/Drill</t>
         </is>

</xml_diff>